<commit_message>
added requirements to test sheet
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Trevor/Desktop/CEG4110/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\josephsluterbeck\CEG4110_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EBC6A4-5180-6741-9C1C-315443A1781E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31A26EE-6BD1-4FAC-A392-D0B683D4C862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="28640" windowHeight="15540" xr2:uid="{037B2FE2-6C72-4D73-B057-C3823F9830A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{037B2FE2-6C72-4D73-B057-C3823F9830A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="37">
   <si>
     <t>RequirementID</t>
   </si>
@@ -118,6 +118,36 @@
   </si>
   <si>
     <t>Trevor</t>
+  </si>
+  <si>
+    <t>Create Shopping Cart</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Edit Shopping Cart</t>
+  </si>
+  <si>
+    <t>Delete Shopping Cart</t>
+  </si>
+  <si>
+    <t>Display Shopping Carts</t>
+  </si>
+  <si>
+    <t>Sign Up as a New User</t>
+  </si>
+  <si>
+    <t>Login as an Existing User</t>
+  </si>
+  <si>
+    <t>Display Recipes&amp;Carts on Profile Page</t>
+  </si>
+  <si>
+    <t>Persistent Data between Logins</t>
   </si>
 </sst>
 </file>
@@ -498,25 +528,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB2A08D0-F8D4-45BB-AA0C-27F01BE068C9}">
-  <dimension ref="B2:I11"/>
+  <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
-    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" customWidth="1"/>
+    <col min="4" max="4" width="46.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -542,7 +572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -562,7 +592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -582,7 +612,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -602,7 +632,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -622,7 +652,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>5</v>
       </c>
@@ -642,7 +672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>6</v>
       </c>
@@ -662,7 +692,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>7</v>
       </c>
@@ -682,7 +712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>8</v>
       </c>
@@ -702,7 +732,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>9</v>
       </c>
@@ -720,6 +750,214 @@
       </c>
       <c r="I11" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="3">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="3">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="3">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="3">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="3">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="3">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="3">
+        <v>7</v>
+      </c>
+      <c r="I18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="3">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="3">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -736,20 +974,20 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
fixed arrow issues, updated testing document
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Trevor/Desktop/CEG4110/CEG4110_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FFADF2-7C29-F246-82BB-00DA0B7AFD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0A52C6-FDD5-784C-B3A1-BAE9F9E48AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28120" windowHeight="14060" xr2:uid="{037B2FE2-6C72-4D73-B057-C3823F9830A0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
   <si>
     <t>RequirementID</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Persistent Data between Logins</t>
+  </si>
+  <si>
+    <t>Recipe Unit Conversion</t>
+  </si>
+  <si>
+    <t>Braden/Trevor</t>
   </si>
 </sst>
 </file>
@@ -528,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB2A08D0-F8D4-45BB-AA0C-27F01BE068C9}">
-  <dimension ref="B2:I19"/>
+  <dimension ref="B2:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -683,7 +689,13 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
       <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
         <v>26</v>
       </c>
       <c r="G7" t="s">
@@ -988,6 +1000,26 @@
       </c>
       <c r="I19" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="3">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="3">
+        <v>6</v>
+      </c>
+      <c r="I20" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>